<commit_message>
stguller2 stage-1 A1 to A6 evidence
</commit_message>
<xml_diff>
--- a/stguller2/evidence.xlsx
+++ b/stguller2/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A748C953-C620-E84E-9E96-81FE25D35129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEDE9D0-8020-3C42-815E-3B00B3F567CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="41">
   <si>
     <t>TxHash</t>
   </si>
@@ -79,24 +79,6 @@
     <t>nft id</t>
   </si>
   <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -143,13 +125,55 @@
   </si>
   <si>
     <t>uptick1hg7qhxqt0l95k4yzyvnljwph8lzga9zlgeznq5</t>
+  </si>
+  <si>
+    <t>746DD641C522F91E347F6920A2A16323640028B419C0635767FAB3360638AC3C</t>
+  </si>
+  <si>
+    <t>nft1</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>sg1</t>
+  </si>
+  <si>
+    <t>8A0DC1123B994B9541C062A3CED986CB1CE16DC21170F2A1372730771B83D680</t>
+  </si>
+  <si>
+    <t>79E2A6B5A67B824463FEB5205879244E06E6A75CDD8F95C1479E3E78520B22B3</t>
+  </si>
+  <si>
+    <t>juno1lqpnudr4k26m9064pw9f25acl370nnkcwq9vsd32sx6urfxejj0qnmmuc2</t>
+  </si>
+  <si>
+    <t>19715F1FEFFA76D5F1633CAB7C353328662262BD978658B0EBB872D9C79F3BF6</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>7ED7EFB032B006A9F5016CF87330B35FCDBD27113043C31995595CE31D3FA53A</t>
+  </si>
+  <si>
+    <t>nft2</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>C975D907FD3B9275BA0995E2266190825B7094B9181F6D446537021182FC1219</t>
+  </si>
+  <si>
+    <t>E285FD4EC0C8FA418ACC8ABE3C3D6992056532D216DD7FBBB5D197A77FCCF043</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +191,33 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF1B1F23"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1B1F23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1B1F23"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -233,8 +284,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -242,6 +291,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -550,71 +607,71 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="43.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -636,8 +693,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -672,8 +729,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -708,8 +765,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -744,8 +801,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -780,8 +837,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -804,13 +861,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -828,8 +883,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -852,13 +907,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -876,8 +929,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -900,13 +953,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -924,8 +975,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -948,13 +999,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -972,8 +1021,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -996,13 +1045,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1020,8 +1067,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1044,13 +1091,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1064,11 +1109,14 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1080,11 +1128,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
+      <c r="A2" t="s">
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1103,8 +1151,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1127,13 +1175,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1151,8 +1197,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1175,13 +1221,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1199,7 +1243,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1233,7 +1277,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1267,7 +1311,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1301,7 +1345,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1329,14 +1373,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="68.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1351,15 +1398,18 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
+      <c r="A2" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1371,15 +1421,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1397,18 +1450,21 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1420,15 +1476,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="66.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1446,18 +1505,21 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="D3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1471,13 +1533,16 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1495,17 +1560,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
+      <c r="A2" t="s">
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1520,14 +1585,15 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1545,17 +1611,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1574,8 +1640,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1610,8 +1676,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
stguller2 Stage-2 C1 to C4 evidence
</commit_message>
<xml_diff>
--- a/stguller2/evidence.xlsx
+++ b/stguller2/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEDE9D0-8020-3C42-815E-3B00B3F567CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8F3843-C4EA-024B-8AD2-A7A063D39623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,8 @@
     <sheet name="A16" sheetId="17" r:id="rId17"/>
     <sheet name="A17" sheetId="18" r:id="rId18"/>
     <sheet name="A18" sheetId="19" r:id="rId19"/>
-    <sheet name="A19" sheetId="20" r:id="rId20"/>
-    <sheet name="A20" sheetId="21" r:id="rId21"/>
+    <sheet name="A19" sheetId="26" r:id="rId20"/>
+    <sheet name="A20" sheetId="20" r:id="rId21"/>
     <sheet name="B1" sheetId="22" r:id="rId22"/>
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="92">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -167,13 +152,181 @@
   </si>
   <si>
     <t>E285FD4EC0C8FA418ACC8ABE3C3D6992056532D216DD7FBBB5D197A77FCCF043</t>
+  </si>
+  <si>
+    <t>nft7</t>
+  </si>
+  <si>
+    <t>B062D84EF4D3CE7D9AAC5058FBE1FBB4A3C5E958B1B23152C7276AA6A0EF21B1</t>
+  </si>
+  <si>
+    <t>nft8</t>
+  </si>
+  <si>
+    <t>4BD3ADEE8DCE4AC59DB1E0A94AD39EEE800CA0FE7E299FCDB0FC7D675E7A9A97</t>
+  </si>
+  <si>
+    <t>nft9</t>
+  </si>
+  <si>
+    <t>ibc/9F10ECE2F5B785B9436EBFE2215BD9FEDD02C0F9564613567094E80CDB4DAE01</t>
+  </si>
+  <si>
+    <t>nft11</t>
+  </si>
+  <si>
+    <t>ibc/67882F729EE670738A1604D9364A9F76214641170E9FEF2B6264F27483B50DF2</t>
+  </si>
+  <si>
+    <t>nft13</t>
+  </si>
+  <si>
+    <t>ibc/E79408F14FE68DD47499F3706869E2D08DF64D5729A712127CA5CEF38BB5534B</t>
+  </si>
+  <si>
+    <t>nft14</t>
+  </si>
+  <si>
+    <t>ibc/FD7CD24223F854AE630544FBC195FB47B1B8FF3FD88BF40F1F9086FBC1E2F306</t>
+  </si>
+  <si>
+    <t>E98D12087D4D50B3A544EB26449D6486D1E866ADB6F30501022C993235EDF151</t>
+  </si>
+  <si>
+    <t>GON-IRISHUB-1</t>
+  </si>
+  <si>
+    <t>219FD4C14068EAA374537D77E2989CDCE197ED91E944916B573FDC305D0BDAB7</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>3704FFD94CC39D57DFB6F9FC53C549E5AB1ADABDD62363CBC1EE5F802820824E</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>4F45C84A62EDD94F49A70357FDB5F5446E6E8C8B762129DD9670DA4F98AFFDB9</t>
+  </si>
+  <si>
+    <t>04AA25EB6E2983668DFA5B1DBBDDF5620EBA7BA636BA089CC83FD05248B04B1D</t>
+  </si>
+  <si>
+    <t>41675BEA99EBA1E10C179BCAF80F8714DB5D10A60501687E0E368FD3F195F6C7</t>
+  </si>
+  <si>
+    <t>C48D2320DBCA753A834D11B841409B978337544B7DECC093F796CA74408B1200</t>
+  </si>
+  <si>
+    <t>5EEF153A9C585258502A7C067D51D2610FF8066DE6A3101084A02109A75F0EA1</t>
+  </si>
+  <si>
+    <t>8BF8E6AFBE2258731048D4587BD69A4D98C1BA5A7245E21B9CE9FEDE837A9321</t>
+  </si>
+  <si>
+    <t>7CD8BDF6E9132B61A988C9CF9FA8BC474CDA8655FCE5B2F57E3773DB065A0403</t>
+  </si>
+  <si>
+    <t>uni-5</t>
+  </si>
+  <si>
+    <t>C58AF85B15B1AC5329A82FB42A387F795F65808F5C0F99AFEAD81C8B56C3C890</t>
+  </si>
+  <si>
+    <t>16028C37BA684A514D8F909D72B29D18AAAB65DC2C4E7E88F136CB6652AF75AC</t>
+  </si>
+  <si>
+    <t>D429B6C45D309DF4EC82DB45DC1156B15DFC18B6F289D622FE08B257B1D9ED33</t>
+  </si>
+  <si>
+    <t>172DA10BDDFBC88EF7EA1AE5FA065D63EE9494A3F8F436867D4328198704EAC9</t>
+  </si>
+  <si>
+    <t>un-5</t>
+  </si>
+  <si>
+    <t>F56287120AFC8F54654FFD8C9F1E6C4628E333198315150B1BE921A7EEC0BD65</t>
+  </si>
+  <si>
+    <t>37C9D55FE84A12C203B6758D31DD3B607817EB7166361749333D94D3085BB04D</t>
+  </si>
+  <si>
+    <t>E049CF964704574E17DBA182BF5919D9F48648DA5D4DE1A5D67055C52D47E397</t>
+  </si>
+  <si>
+    <t>09DEA5BB80C755CC6EB5761CDBDDE7E5F9C359F02A4A9B3CE80FA9B45267B884</t>
+  </si>
+  <si>
+    <t>A8D870E7AEC23B635CFA66EF17B72FCDF57A4A7BDB9CECD23D62D466AED87E1B</t>
+  </si>
+  <si>
+    <t>2A6398A8DC6B9A84453B4C3D40815FB0FC65C8C09B469209CF6AA8F6D96A76A0</t>
+  </si>
+  <si>
+    <t>5338FA8116879359E028677B01ACD72F9B36AAE0A584BA5F8E2E503676E9E0C1</t>
+  </si>
+  <si>
+    <t>EFE937302A6634BEF41139C505E7A249A2B82AB1D9AFB264DE3FDA4E7631160B</t>
+  </si>
+  <si>
+    <t>3E23561B53C4D8E7A96FB6EF0629BDE07748FC3613C8E82EA31B2CFA4146C971</t>
+  </si>
+  <si>
+    <t>859E25A32EF3BAADF514CD1AEF958431A0E73EC11205B4CC7309D55633F76D42</t>
+  </si>
+  <si>
+    <t>EF924C92B2DECCEBE5964D71BEEF021DB96B6B4D4E9BBE9D80EAD11CC9DA8D3D</t>
+  </si>
+  <si>
+    <t>EE5BD8B148695677961DD18439A294AFA4C0042F2F278AF0744B029547303A6F</t>
+  </si>
+  <si>
+    <t>413D2AA5BA9BBC58B4843F6BEDED5569E5EC4473719BFA76B851014E6EF8BEB9</t>
+  </si>
+  <si>
+    <t>0697942C038DD33CD70757CEED8FE7628D4C6481997DE1E5B4A98A8682374F8C</t>
+  </si>
+  <si>
+    <t>uptick-7000-2</t>
+  </si>
+  <si>
+    <t>019BAA2BC3DB9113212C0BBC86300D79A289642278551823DD38B5372198D673</t>
+  </si>
+  <si>
+    <t>8FD9A513C2F15A31196EFEBE9E2655FA52E14D743A3A75F8AD5225B88FBD08EC</t>
+  </si>
+  <si>
+    <t>23F377ECC34ED7F3126B264A4775C32DAF5DFC4F48019F7D0542A532F5D3BA28</t>
+  </si>
+  <si>
+    <t>8F4E773EBA2D584EA429D9D13F3E8EAC4C6C8C30A3BDCA4581C338E44A805E7E</t>
+  </si>
+  <si>
+    <t>UPTICK_7000-2</t>
+  </si>
+  <si>
+    <t>13E91418878C39692F5C86FB98E89AC1962F34925C509F9CD7F54E32E79BDC10</t>
+  </si>
+  <si>
+    <t>2BC3BDEB0C2B12AE24D49E631F94C1B20638A9EA9C1F9040A8C0B3FD6C63CA20</t>
+  </si>
+  <si>
+    <t>GON-FLIXNET-1</t>
+  </si>
+  <si>
+    <t>2B31558B1F497483E64BA69C175541CC636FE9FC4809ADF990B9F39D5F83C3B7</t>
+  </si>
+  <si>
+    <t>1093CF6BE533B0C3817CC0751672AA04560E08AD7F35BFF5429B5F85BF7DD0EA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +371,32 @@
     <font>
       <sz val="11"/>
       <color rgb="FF1B1F23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -276,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -293,12 +472,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -624,54 +810,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -689,432 +875,543 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="75.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="117" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="EA126" sqref="EA126"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" location="/transactions/7CD8BDF6E9132B61A988C9CF9FA8BC474CDA8655FCE5B2F57E3773DB065A0403" display="https://blueprints.juno.giansalex.dev/ - /transactions/7CD8BDF6E9132B61A988C9CF9FA8BC474CDA8655FCE5B2F57E3773DB065A0403" xr:uid="{5AEAECB4-01E4-2D4C-AA5D-FA93E22CC6A7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="69.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
     <col min="1" max="1" width="65.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1124,35 +1421,115 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B36147D-C5A1-1744-9EAE-0367DCD9AB66}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="75.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1165,66 +1542,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>85</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>87</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1391,21 +1752,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
@@ -1440,27 +1801,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>29</v>
+      <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
@@ -1495,27 +1856,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>38</v>
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
@@ -1534,7 +1895,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1550,10 +1911,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1561,16 +1922,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1585,7 +1946,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1601,27 +1962,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>35</v>
+      <c r="A2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1636,28 +1997,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1672,28 +2035,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved format error Stage 1 and Stage 2 (A1-A20)
</commit_message>
<xml_diff>
--- a/stguller2/evidence.xlsx
+++ b/stguller2/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8F3843-C4EA-024B-8AD2-A7A063D39623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996B49DD-5451-A948-AF4C-BCB8DD87DC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" firstSheet="8" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="88">
   <si>
     <t>TxHash</t>
   </si>
@@ -151,9 +151,6 @@
     <t>C975D907FD3B9275BA0995E2266190825B7094B9181F6D446537021182FC1219</t>
   </si>
   <si>
-    <t>E285FD4EC0C8FA418ACC8ABE3C3D6992056532D216DD7FBBB5D197A77FCCF043</t>
-  </si>
-  <si>
     <t>nft7</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>E98D12087D4D50B3A544EB26449D6486D1E866ADB6F30501022C993235EDF151</t>
   </si>
   <si>
-    <t>GON-IRISHUB-1</t>
-  </si>
-  <si>
     <t>219FD4C14068EAA374537D77E2989CDCE197ED91E944916B573FDC305D0BDAB7</t>
   </si>
   <si>
@@ -229,9 +223,6 @@
     <t>7CD8BDF6E9132B61A988C9CF9FA8BC474CDA8655FCE5B2F57E3773DB065A0403</t>
   </si>
   <si>
-    <t>uni-5</t>
-  </si>
-  <si>
     <t>C58AF85B15B1AC5329A82FB42A387F795F65808F5C0F99AFEAD81C8B56C3C890</t>
   </si>
   <si>
@@ -244,9 +235,6 @@
     <t>172DA10BDDFBC88EF7EA1AE5FA065D63EE9494A3F8F436867D4328198704EAC9</t>
   </si>
   <si>
-    <t>un-5</t>
-  </si>
-  <si>
     <t>F56287120AFC8F54654FFD8C9F1E6C4628E333198315150B1BE921A7EEC0BD65</t>
   </si>
   <si>
@@ -289,9 +277,6 @@
     <t>0697942C038DD33CD70757CEED8FE7628D4C6481997DE1E5B4A98A8682374F8C</t>
   </si>
   <si>
-    <t>uptick-7000-2</t>
-  </si>
-  <si>
     <t>019BAA2BC3DB9113212C0BBC86300D79A289642278551823DD38B5372198D673</t>
   </si>
   <si>
@@ -304,29 +289,32 @@
     <t>8F4E773EBA2D584EA429D9D13F3E8EAC4C6C8C30A3BDCA4581C338E44A805E7E</t>
   </si>
   <si>
-    <t>UPTICK_7000-2</t>
-  </si>
-  <si>
     <t>13E91418878C39692F5C86FB98E89AC1962F34925C509F9CD7F54E32E79BDC10</t>
   </si>
   <si>
     <t>2BC3BDEB0C2B12AE24D49E631F94C1B20638A9EA9C1F9040A8C0B3FD6C63CA20</t>
   </si>
   <si>
-    <t>GON-FLIXNET-1</t>
-  </si>
-  <si>
     <t>2B31558B1F497483E64BA69C175541CC636FE9FC4809ADF990B9F39D5F83C3B7</t>
   </si>
   <si>
     <t>1093CF6BE533B0C3817CC0751672AA04560E08AD7F35BFF5429B5F85BF7DD0EA</t>
+  </si>
+  <si>
+    <t>ibc/E285FD4EC0C8FA418ACC8ABE3C3D6992056532D216DD7FBBB5D197A77FCCF043</t>
+  </si>
+  <si>
+    <t>nft0</t>
+  </si>
+  <si>
+    <t>C2D390DE87C588C91B3141142B37460CF11FADB2840CAEC7E9D8BE19449537D0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,24 +364,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -455,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -463,13 +438,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -477,13 +448,23 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -793,8 +774,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="81" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -802,7 +783,7 @@
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
@@ -834,29 +815,29 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -876,7 +857,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -893,12 +874,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>40</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -914,127 +895,189 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="75.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="165" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="72.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="74.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="75.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="74" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1045,35 +1088,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1082,21 +1125,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="117" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="EA126" sqref="EA126"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1107,98 +1150,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="74.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B4" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
+      <c r="B5" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1198,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1234,36 +1215,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
+      <c r="B5" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1279,13 +1260,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="74.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1296,40 +1277,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>51</v>
+    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
+      <c r="A6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1344,12 +1325,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1361,40 +1342,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1406,9 +1387,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1424,11 +1403,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1445,7 +1424,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1462,52 +1441,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>51</v>
+      <c r="B7" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1522,13 +1501,13 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1540,52 +1519,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1736,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1758,19 +1737,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+    <row r="3" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1785,7 +1772,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1810,22 +1797,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:4" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1840,13 +1827,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="66.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -1865,22 +1852,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="D3" s="6"/>
+      <c r="D3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1895,7 +1882,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1920,18 +1907,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>30</v>
+      <c r="D2" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1947,12 +1934,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1971,18 +1959,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1998,7 +1986,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2015,12 +2003,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>36</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2036,7 +2024,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2053,13 +2041,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
stguller2 Solved format error Stage 1_Stage 2 (A1-A20)
Solved format error Stage 1 and Stage 2 (A1-A20) and reported "A4: Tx: result is unachievable" error fixed.
</commit_message>
<xml_diff>
--- a/stguller2/evidence.xlsx
+++ b/stguller2/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996B49DD-5451-A948-AF4C-BCB8DD87DC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E269A4-BC68-B947-BA9D-BAEBAF476D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" firstSheet="8" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -461,9 +461,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -815,7 +814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -874,7 +873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -912,7 +911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>42</v>
       </c>
@@ -950,7 +949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>44</v>
       </c>
@@ -988,7 +987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>46</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>47</v>
       </c>
@@ -1034,7 +1033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>48</v>
       </c>
@@ -1042,7 +1041,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>50</v>
       </c>
@@ -1050,7 +1049,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>52</v>
       </c>
@@ -1088,7 +1087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>53</v>
       </c>
@@ -1096,7 +1095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
@@ -1104,7 +1103,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>55</v>
       </c>
@@ -1112,7 +1111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>56</v>
       </c>
@@ -1150,7 +1149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>57</v>
       </c>
@@ -1158,27 +1157,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1215,35 +1214,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1277,35 +1276,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1342,7 +1341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>69</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>70</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>71</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>72</v>
       </c>
@@ -1441,7 +1440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>73</v>
       </c>
@@ -1449,7 +1448,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>74</v>
       </c>
@@ -1457,7 +1456,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>75</v>
       </c>
@@ -1465,7 +1464,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>76</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>77</v>
       </c>
@@ -1481,7 +1480,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>78</v>
       </c>
@@ -1501,7 +1500,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -1519,7 +1518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>79</v>
       </c>
@@ -1527,7 +1526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>80</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>81</v>
       </c>
@@ -1543,7 +1542,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>82</v>
       </c>
@@ -1551,7 +1550,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>83</v>
       </c>
@@ -1559,7 +1558,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>84</v>
       </c>
@@ -1737,7 +1736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>87</v>
       </c>
@@ -1797,11 +1796,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -1826,15 +1825,15 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="66.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1852,8 +1851,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1863,7 +1862,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
@@ -1907,8 +1906,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1959,7 +1958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
@@ -1969,7 +1968,7 @@
       <c r="C2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2003,7 +2002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>36</v>
       </c>
@@ -2041,7 +2040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
stguller2 add stage-3 B1-B2
</commit_message>
<xml_diff>
--- a/stguller2/evidence.xlsx
+++ b/stguller2/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E269A4-BC68-B947-BA9D-BAEBAF476D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308BEDF8-BC8B-1542-B7E8-B4E60E1BDA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" firstSheet="9" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="92">
   <si>
     <t>TxHash</t>
   </si>
@@ -308,6 +308,18 @@
   </si>
   <si>
     <t>C2D390DE87C588C91B3141142B37460CF11FADB2840CAEC7E9D8BE19449537D0</t>
+  </si>
+  <si>
+    <t>721FECB35598A390E92659848A7C7D55BAE2504748173EB02E22CE678B877E76</t>
+  </si>
+  <si>
+    <t>E97E1C1F81926FB07A7FEEB3483BE58CC4456A4468DCA1DFFB965F6552B43091</t>
+  </si>
+  <si>
+    <t>FBAB86A707514C51B7EC6206A36C915ECE68DB9A47F6A89E24FDA1B1AC2D634A</t>
+  </si>
+  <si>
+    <t>B10DE0190BCB0D4779CA0D03CF4BEA6FD20ED34B2EE284612823F78A02D9E6CF</t>
   </si>
 </sst>
 </file>
@@ -1501,7 +1513,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1578,11 +1590,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1592,12 +1606,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1612,11 +1626,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1626,12 +1642,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1841,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>